<commit_message>
fórmula de limites atualizada
</commit_message>
<xml_diff>
--- a/contratos.xlsx
+++ b/contratos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raoni\OneDrive\Área de Trabalho\projetos-python\spreads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AFFC22-6272-4658-9938-4FEBF560CFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7D8E76-FA0B-45B9-A8F1-EBFF8D99C33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{45C0CBED-74D7-4461-A86C-E6BB91E36BC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{45C0CBED-74D7-4461-A86C-E6BB91E36BC4}"/>
   </bookViews>
   <sheets>
     <sheet name="indicadores" sheetId="4" r:id="rId1"/>
@@ -6468,7 +6468,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0968EECD-0D54-4DF8-8453-31DD28DF051A}">
   <dimension ref="A1:T5002"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6590,7 +6592,7 @@
         <v>23</v>
       </c>
       <c r="N2" s="11">
-        <f>_xlfn.QUARTILE.EXC($C$2:$C$6,1)</f>
+        <f>_xlfn.QUARTILE.INC($C$2:$C$6,1)</f>
         <v>0.04</v>
       </c>
       <c r="O2" s="6"/>
@@ -6770,8 +6772,8 @@
         <v>25</v>
       </c>
       <c r="N5" s="10">
-        <f>$N$1+1.5*N4</f>
-        <v>5.4333333333333338E-2</v>
+        <f>$N$3+1.5*N4</f>
+        <v>5.6666666666666671E-2</v>
       </c>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
@@ -6825,8 +6827,8 @@
         <v>26</v>
       </c>
       <c r="N6" s="10">
-        <f>N1-1.5*N4</f>
-        <v>3.4333333333333334E-2</v>
+        <f>N2-1.5*N4</f>
+        <v>0.03</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>

</xml_diff>